<commit_message>
Added placeholders for elevator info
</commit_message>
<xml_diff>
--- a/AIAD/src/assets/statistics.xlsx
+++ b/AIAD/src/assets/statistics.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
   <si>
     <t>Wait time</t>
   </si>
@@ -65,13 +65,22 @@
     <t>elev0</t>
   </si>
   <si>
+    <t>DOWN</t>
+  </si>
+  <si>
+    <t>NO_DIRECTION</t>
+  </si>
+  <si>
     <t>UP</t>
   </si>
   <si>
-    <t>NO_DIRECTION</t>
-  </si>
-  <si>
-    <t>DOWN</t>
+    <t>elev1</t>
+  </si>
+  <si>
+    <t>elev2</t>
+  </si>
+  <si>
+    <t>elev3</t>
   </si>
 </sst>
 </file>
@@ -127,7 +136,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:Y17"/>
+  <dimension ref="B2:Y20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -148,10 +157,10 @@
     </row>
     <row r="4">
       <c r="B4" t="n">
-        <v>430.0</v>
+        <v>887.0</v>
       </c>
       <c r="C4" t="n">
-        <v>9897.0</v>
+        <v>3418.0</v>
       </c>
     </row>
     <row r="6">
@@ -226,6 +235,15 @@
       </c>
     </row>
     <row r="7">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0</v>
+      </c>
       <c r="F7" t="n">
         <v>0.0</v>
       </c>
@@ -233,7 +251,7 @@
         <v>16</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I7" t="n">
         <v>0.0</v>
@@ -245,13 +263,13 @@
         <v>18</v>
       </c>
       <c r="L7" t="n">
-        <v>1.512915536315E12</v>
+        <v>1.512917502335E12</v>
       </c>
       <c r="M7" t="n">
-        <v>1.512915536745E12</v>
+        <v>1.512917503222E12</v>
       </c>
       <c r="N7" t="n">
-        <v>430.0</v>
+        <v>887.0</v>
       </c>
       <c r="P7" t="n">
         <v>0.0</v>
@@ -260,54 +278,63 @@
         <v>16</v>
       </c>
       <c r="R7" t="n">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
       <c r="S7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="T7" t="s">
+        <v>19</v>
+      </c>
+      <c r="U7" t="s">
+        <v>19</v>
+      </c>
+      <c r="V7" t="n">
+        <v>1.512917503222E12</v>
+      </c>
+      <c r="W7" t="n">
+        <v>1.512917505101E12</v>
+      </c>
+      <c r="X7" t="n">
+        <v>1879.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" t="s">
         <v>18</v>
       </c>
-      <c r="U7" t="s">
-        <v>18</v>
-      </c>
-      <c r="V7" t="n">
-        <v>1.512915536745E12</v>
-      </c>
-      <c r="W7" t="n">
-        <v>1.51291554419E12</v>
-      </c>
-      <c r="X7" t="n">
-        <v>7445.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="F8" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" t="s">
-        <v>17</v>
-      </c>
       <c r="L8" t="n">
-        <v>1.512915538297E12</v>
+        <v>1.512917502784E12</v>
       </c>
       <c r="M8" t="n">
-        <v>1.512915545693E12</v>
+        <v>1.512917506202E12</v>
       </c>
       <c r="N8" t="n">
-        <v>7396.0</v>
+        <v>3418.0</v>
       </c>
       <c r="P8" t="n">
         <v>1.0</v>
@@ -316,28 +343,64 @@
         <v>16</v>
       </c>
       <c r="R8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T8" t="s">
+        <v>19</v>
+      </c>
+      <c r="U8" t="s">
+        <v>19</v>
+      </c>
+      <c r="V8" t="n">
+        <v>1.512917503222E12</v>
+      </c>
+      <c r="W8" t="n">
+        <v>1.512917505101E12</v>
+      </c>
+      <c r="X8" t="n">
+        <v>1879.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F9" t="n">
         <v>2.0</v>
       </c>
-      <c r="S8" t="n">
-        <v>11.0</v>
-      </c>
-      <c r="T8" t="s">
-        <v>19</v>
-      </c>
-      <c r="U8" t="s">
-        <v>19</v>
-      </c>
-      <c r="V8" t="n">
-        <v>1.512915545693E12</v>
-      </c>
-      <c r="W8" t="n">
-        <v>1.512915551206E12</v>
-      </c>
-      <c r="X8" t="n">
-        <v>5513.0</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1.512917504815E12</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1.512917508209E12</v>
+      </c>
+      <c r="N9" t="n">
+        <v>3394.0</v>
+      </c>
       <c r="P9" t="n">
         <v>2.0</v>
       </c>
@@ -345,10 +408,10 @@
         <v>16</v>
       </c>
       <c r="R9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="S9" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="T9" t="s">
         <v>19</v>
@@ -357,16 +420,25 @@
         <v>19</v>
       </c>
       <c r="V9" t="n">
-        <v>1.512915550204E12</v>
+        <v>1.512917503222E12</v>
       </c>
       <c r="W9" t="n">
-        <v>1.512915552208E12</v>
+        <v>1.512917505101E12</v>
       </c>
       <c r="X9" t="n">
-        <v>2004.0</v>
+        <v>1879.0</v>
       </c>
     </row>
     <row r="10">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0</v>
+      </c>
       <c r="P10" t="n">
         <v>3.0</v>
       </c>
@@ -377,7 +449,7 @@
         <v>0.0</v>
       </c>
       <c r="S10" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="T10" t="s">
         <v>19</v>
@@ -386,13 +458,13 @@
         <v>19</v>
       </c>
       <c r="V10" t="n">
-        <v>1.512915550204E12</v>
+        <v>1.512917503222E12</v>
       </c>
       <c r="W10" t="n">
-        <v>1.51291555321E12</v>
+        <v>1.512917505101E12</v>
       </c>
       <c r="X10" t="n">
-        <v>3006.0</v>
+        <v>1879.0</v>
       </c>
     </row>
     <row r="11">
@@ -400,13 +472,13 @@
         <v>4.0</v>
       </c>
       <c r="Q11" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="R11" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="S11" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="T11" t="s">
         <v>19</v>
@@ -415,13 +487,13 @@
         <v>19</v>
       </c>
       <c r="V11" t="n">
-        <v>1.512915550204E12</v>
+        <v>1.512917506202E12</v>
       </c>
       <c r="W11" t="n">
-        <v>1.512915552208E12</v>
+        <v>1.512917507706E12</v>
       </c>
       <c r="X11" t="n">
-        <v>2004.0</v>
+        <v>1504.0</v>
       </c>
     </row>
     <row r="12">
@@ -429,13 +501,13 @@
         <v>5.0</v>
       </c>
       <c r="Q12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="R12" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="S12" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="T12" t="s">
         <v>19</v>
@@ -444,13 +516,13 @@
         <v>19</v>
       </c>
       <c r="V12" t="n">
-        <v>1.512915550204E12</v>
+        <v>1.512917506202E12</v>
       </c>
       <c r="W12" t="n">
-        <v>1.51291555321E12</v>
+        <v>1.512917507706E12</v>
       </c>
       <c r="X12" t="n">
-        <v>3006.0</v>
+        <v>1504.0</v>
       </c>
     </row>
     <row r="13">
@@ -458,13 +530,13 @@
         <v>6.0</v>
       </c>
       <c r="Q13" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="R13" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="S13" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="T13" t="s">
         <v>19</v>
@@ -473,100 +545,158 @@
         <v>19</v>
       </c>
       <c r="V13" t="n">
-        <v>1.512915550204E12</v>
+        <v>1.512917506202E12</v>
       </c>
       <c r="W13" t="n">
-        <v>1.51291555321E12</v>
+        <v>1.512917509209E12</v>
       </c>
       <c r="X13" t="n">
+        <v>3007.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="P14" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>19</v>
+      </c>
+      <c r="U14" t="s">
+        <v>19</v>
+      </c>
+      <c r="V14" t="n">
+        <v>1.512917506202E12</v>
+      </c>
+      <c r="W14" t="n">
+        <v>1.512917510211E12</v>
+      </c>
+      <c r="X14" t="n">
+        <v>4009.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="P15" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>20</v>
+      </c>
+      <c r="R15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>19</v>
+      </c>
+      <c r="U15" t="s">
+        <v>19</v>
+      </c>
+      <c r="V15" t="n">
+        <v>1.512917506202E12</v>
+      </c>
+      <c r="W15" t="n">
+        <v>1.512917510211E12</v>
+      </c>
+      <c r="X15" t="n">
+        <v>4009.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="P18" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>21</v>
+      </c>
+      <c r="R18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="T18" t="s">
+        <v>19</v>
+      </c>
+      <c r="U18" t="s">
+        <v>19</v>
+      </c>
+      <c r="V18" t="n">
+        <v>1.512917508209E12</v>
+      </c>
+      <c r="W18" t="n">
+        <v>1.512917511215E12</v>
+      </c>
+      <c r="X18" t="n">
         <v>3006.0</v>
       </c>
     </row>
-    <row r="14">
-      <c r="F14" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I14" t="n">
+    <row r="19">
+      <c r="P19" t="n">
         <v>12.0</v>
       </c>
-      <c r="J14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" t="s">
-        <v>17</v>
-      </c>
-      <c r="L14" t="n">
-        <v>1.512915543313E12</v>
-      </c>
-      <c r="M14" t="n">
-        <v>1.51291555321E12</v>
-      </c>
-      <c r="N14" t="n">
-        <v>9897.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="P16" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R16" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="T16" t="s">
-        <v>19</v>
-      </c>
-      <c r="U16" t="s">
-        <v>19</v>
-      </c>
-      <c r="V16" t="n">
-        <v>1.51291555321E12</v>
-      </c>
-      <c r="W16" t="n">
-        <v>1.512915558222E12</v>
-      </c>
-      <c r="X16" t="n">
-        <v>5012.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="F17" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="G17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="I17" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="J17" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" t="n">
-        <v>1.512915547823E12</v>
-      </c>
-      <c r="M17" t="n">
-        <v>1.512915550204E12</v>
-      </c>
-      <c r="N17" t="n">
-        <v>2381.0</v>
+      <c r="Q19" t="s">
+        <v>21</v>
+      </c>
+      <c r="R19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="T19" t="s">
+        <v>19</v>
+      </c>
+      <c r="U19" t="s">
+        <v>19</v>
+      </c>
+      <c r="V19" t="n">
+        <v>1.512917508209E12</v>
+      </c>
+      <c r="W19" t="n">
+        <v>1.512917511215E12</v>
+      </c>
+      <c r="X19" t="n">
+        <v>3006.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="P20" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>21</v>
+      </c>
+      <c r="R20" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="T20" t="s">
+        <v>19</v>
+      </c>
+      <c r="U20" t="s">
+        <v>19</v>
+      </c>
+      <c r="V20" t="n">
+        <v>1.512917508209E12</v>
+      </c>
+      <c r="W20" t="n">
+        <v>1.512917511215E12</v>
+      </c>
+      <c r="X20" t="n">
+        <v>3006.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>